<commit_message>
Se modifica los services de status y location para enviar  los datos al frontend
</commit_message>
<xml_diff>
--- a/src/main/resources/static/FO-GTI-01.xlsx
+++ b/src/main/resources/static/FO-GTI-01.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cristian\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Inventario TI\inventory_system\src\main\resources\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62610DD7-8D53-4180-8061-283058C61361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7EA946-DB83-47EF-9FCD-2F4772B7DAD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" tabRatio="267" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="267" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>DATOS</t>
   </si>
@@ -157,9 +157,6 @@
   </si>
   <si>
     <t>CALI</t>
-  </si>
-  <si>
-    <t>GESTION TI</t>
   </si>
   <si>
     <t>Aprendiz Sist. De Inf.</t>
@@ -1095,37 +1092,43 @@
     <xf numFmtId="3" fontId="8" fillId="4" borderId="53" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1140,67 +1143,94 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1287,111 +1317,78 @@
     <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Millares" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1779,10 +1776,10 @@
   <dimension ref="B1:L40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29:K29"/>
+      <selection activeCell="D8" sqref="D8:K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="21.6640625" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="21.6640625" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="0.5546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.33203125" style="1" customWidth="1"/>
@@ -1812,45 +1809,45 @@
       <c r="K1" s="2"/>
     </row>
     <row r="2" spans="2:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="88"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="68" t="s">
+      <c r="B2" s="99"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="70"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="81"/>
       <c r="K2" s="29" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="2:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="90"/>
-      <c r="C3" s="91"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="73"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="102"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="83"/>
+      <c r="G3" s="83"/>
+      <c r="H3" s="83"/>
+      <c r="I3" s="83"/>
+      <c r="J3" s="84"/>
       <c r="K3" s="30" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="92"/>
-      <c r="C4" s="93"/>
-      <c r="D4" s="74"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75"/>
-      <c r="J4" s="76"/>
+      <c r="B4" s="103"/>
+      <c r="C4" s="104"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="86"/>
+      <c r="J4" s="87"/>
       <c r="K4" s="31" t="s">
         <v>28</v>
       </c>
@@ -1868,93 +1865,91 @@
       <c r="K5" s="10"/>
     </row>
     <row r="6" spans="2:12" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="77" t="s">
+      <c r="B6" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="78"/>
-      <c r="D6" s="38" t="s">
+      <c r="C6" s="89"/>
+      <c r="D6" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="39"/>
-      <c r="F6" s="110" t="s">
+      <c r="E6" s="77"/>
+      <c r="F6" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="110"/>
-      <c r="H6" s="111"/>
+      <c r="G6" s="69"/>
+      <c r="H6" s="70"/>
       <c r="I6" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="108"/>
-      <c r="K6" s="109"/>
+      <c r="J6" s="67"/>
+      <c r="K6" s="68"/>
     </row>
     <row r="7" spans="2:12" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="79"/>
-      <c r="C7" s="80"/>
-      <c r="D7" s="83" t="s">
+      <c r="B7" s="90"/>
+      <c r="C7" s="91"/>
+      <c r="D7" s="94" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="84"/>
-      <c r="F7" s="84"/>
-      <c r="G7" s="84"/>
-      <c r="H7" s="84"/>
-      <c r="I7" s="84"/>
-      <c r="J7" s="84"/>
-      <c r="K7" s="85"/>
+      <c r="E7" s="95"/>
+      <c r="F7" s="95"/>
+      <c r="G7" s="95"/>
+      <c r="H7" s="95"/>
+      <c r="I7" s="95"/>
+      <c r="J7" s="95"/>
+      <c r="K7" s="96"/>
     </row>
     <row r="8" spans="2:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="81" t="s">
+      <c r="B8" s="92" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="82"/>
-      <c r="D8" s="40" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="42"/>
+      <c r="C8" s="93"/>
+      <c r="D8" s="117"/>
+      <c r="E8" s="118"/>
+      <c r="F8" s="118"/>
+      <c r="G8" s="118"/>
+      <c r="H8" s="118"/>
+      <c r="I8" s="118"/>
+      <c r="J8" s="118"/>
+      <c r="K8" s="119"/>
       <c r="L8" s="4"/>
     </row>
     <row r="9" spans="2:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="94" t="s">
+      <c r="B9" s="105" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="95"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="59"/>
-      <c r="H9" s="59"/>
-      <c r="I9" s="59"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="61"/>
+      <c r="C9" s="106"/>
+      <c r="D9" s="126"/>
+      <c r="E9" s="127"/>
+      <c r="F9" s="127"/>
+      <c r="G9" s="127"/>
+      <c r="H9" s="127"/>
+      <c r="I9" s="127"/>
+      <c r="J9" s="128"/>
+      <c r="K9" s="129"/>
     </row>
     <row r="10" spans="2:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="86" t="s">
+      <c r="B10" s="97" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="87"/>
-      <c r="D10" s="114"/>
-      <c r="E10" s="115"/>
-      <c r="F10" s="115"/>
-      <c r="G10" s="115"/>
-      <c r="H10" s="115"/>
-      <c r="I10" s="116"/>
-      <c r="J10" s="112" t="s">
+      <c r="C10" s="98"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="74"/>
+      <c r="F10" s="74"/>
+      <c r="G10" s="74"/>
+      <c r="H10" s="74"/>
+      <c r="I10" s="75"/>
+      <c r="J10" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="K10" s="113"/>
+      <c r="K10" s="72"/>
     </row>
     <row r="11" spans="2:12" ht="15" x14ac:dyDescent="0.3">
-      <c r="B11" s="99" t="s">
+      <c r="B11" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="100"/>
-      <c r="D11" s="101"/>
-      <c r="E11" s="49" t="s">
+      <c r="C11" s="59"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="122" t="s">
         <v>7</v>
       </c>
       <c r="F11" s="50"/>
@@ -1971,16 +1966,16 @@
       <c r="K11" s="26"/>
     </row>
     <row r="12" spans="2:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="102"/>
-      <c r="C12" s="103"/>
-      <c r="D12" s="104"/>
-      <c r="E12" s="47"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="48"/>
+      <c r="B12" s="61"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="63"/>
+      <c r="E12" s="120"/>
+      <c r="F12" s="121"/>
+      <c r="G12" s="121"/>
+      <c r="H12" s="121"/>
       <c r="I12" s="25"/>
       <c r="J12" s="27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K12" s="28"/>
     </row>
@@ -1996,25 +1991,25 @@
       <c r="J13" s="6"/>
     </row>
     <row r="14" spans="2:12" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="105" t="s">
+      <c r="B14" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="106"/>
-      <c r="D14" s="106"/>
-      <c r="E14" s="106"/>
-      <c r="F14" s="106"/>
-      <c r="G14" s="106"/>
-      <c r="H14" s="106"/>
-      <c r="I14" s="106"/>
-      <c r="J14" s="106"/>
-      <c r="K14" s="107"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="65"/>
+      <c r="I14" s="65"/>
+      <c r="J14" s="65"/>
+      <c r="K14" s="66"/>
     </row>
     <row r="15" spans="2:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="39"/>
-      <c r="D15" s="54"/>
+      <c r="C15" s="77"/>
+      <c r="D15" s="78"/>
       <c r="E15" s="22" t="s">
         <v>18</v>
       </c>
@@ -2024,156 +2019,156 @@
       <c r="G15" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="39" t="s">
+      <c r="H15" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="I15" s="39"/>
-      <c r="J15" s="39"/>
-      <c r="K15" s="54"/>
+      <c r="I15" s="77"/>
+      <c r="J15" s="77"/>
+      <c r="K15" s="78"/>
     </row>
     <row r="16" spans="2:12" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="96"/>
-      <c r="C16" s="97"/>
-      <c r="D16" s="98"/>
+      <c r="B16" s="55"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="57"/>
       <c r="E16" s="17"/>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
-      <c r="H16" s="51"/>
-      <c r="I16" s="52"/>
-      <c r="J16" s="52"/>
-      <c r="K16" s="53"/>
+      <c r="H16" s="123"/>
+      <c r="I16" s="124"/>
+      <c r="J16" s="124"/>
+      <c r="K16" s="125"/>
     </row>
     <row r="17" spans="2:11" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="62"/>
-      <c r="C17" s="63"/>
-      <c r="D17" s="64"/>
+      <c r="B17" s="107"/>
+      <c r="C17" s="108"/>
+      <c r="D17" s="109"/>
       <c r="E17" s="16"/>
       <c r="F17" s="15"/>
       <c r="G17" s="15"/>
-      <c r="H17" s="55"/>
-      <c r="I17" s="56"/>
-      <c r="J17" s="56"/>
-      <c r="K17" s="57"/>
+      <c r="H17" s="110"/>
+      <c r="I17" s="111"/>
+      <c r="J17" s="111"/>
+      <c r="K17" s="112"/>
     </row>
     <row r="18" spans="2:11" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="65"/>
-      <c r="C18" s="66"/>
-      <c r="D18" s="67"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="38"/>
       <c r="E18" s="16"/>
       <c r="F18" s="15"/>
       <c r="G18" s="15"/>
-      <c r="H18" s="55"/>
-      <c r="I18" s="56"/>
-      <c r="J18" s="56"/>
-      <c r="K18" s="57"/>
+      <c r="H18" s="110"/>
+      <c r="I18" s="111"/>
+      <c r="J18" s="111"/>
+      <c r="K18" s="112"/>
     </row>
     <row r="19" spans="2:11" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="65"/>
-      <c r="C19" s="66"/>
-      <c r="D19" s="67"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="38"/>
       <c r="E19" s="16"/>
       <c r="F19" s="15"/>
       <c r="G19" s="15"/>
-      <c r="H19" s="55"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="56"/>
-      <c r="K19" s="57"/>
+      <c r="H19" s="110"/>
+      <c r="I19" s="111"/>
+      <c r="J19" s="111"/>
+      <c r="K19" s="112"/>
     </row>
     <row r="20" spans="2:11" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="65"/>
-      <c r="C20" s="66"/>
-      <c r="D20" s="67"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="38"/>
       <c r="E20" s="16"/>
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>
-      <c r="H20" s="55"/>
-      <c r="I20" s="56"/>
-      <c r="J20" s="56"/>
-      <c r="K20" s="57"/>
+      <c r="H20" s="110"/>
+      <c r="I20" s="111"/>
+      <c r="J20" s="111"/>
+      <c r="K20" s="112"/>
     </row>
     <row r="21" spans="2:11" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="65"/>
-      <c r="C21" s="66"/>
-      <c r="D21" s="67"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="38"/>
       <c r="E21" s="16"/>
       <c r="F21" s="15"/>
       <c r="G21" s="15"/>
-      <c r="H21" s="55"/>
-      <c r="I21" s="56"/>
-      <c r="J21" s="56"/>
-      <c r="K21" s="57"/>
+      <c r="H21" s="110"/>
+      <c r="I21" s="111"/>
+      <c r="J21" s="111"/>
+      <c r="K21" s="112"/>
     </row>
     <row r="22" spans="2:11" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="65"/>
-      <c r="C22" s="66"/>
-      <c r="D22" s="67"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="38"/>
       <c r="E22" s="16"/>
       <c r="F22" s="15"/>
       <c r="G22" s="15"/>
-      <c r="H22" s="55"/>
-      <c r="I22" s="56"/>
-      <c r="J22" s="56"/>
-      <c r="K22" s="57"/>
+      <c r="H22" s="110"/>
+      <c r="I22" s="111"/>
+      <c r="J22" s="111"/>
+      <c r="K22" s="112"/>
     </row>
     <row r="23" spans="2:11" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="65"/>
-      <c r="C23" s="66"/>
-      <c r="D23" s="67"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="38"/>
       <c r="E23" s="16"/>
       <c r="F23" s="15"/>
       <c r="G23" s="15"/>
-      <c r="H23" s="55"/>
-      <c r="I23" s="56"/>
-      <c r="J23" s="56"/>
-      <c r="K23" s="57"/>
+      <c r="H23" s="110"/>
+      <c r="I23" s="111"/>
+      <c r="J23" s="111"/>
+      <c r="K23" s="112"/>
     </row>
     <row r="24" spans="2:11" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="65"/>
-      <c r="C24" s="66"/>
-      <c r="D24" s="67"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="38"/>
       <c r="E24" s="16"/>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
-      <c r="H24" s="55"/>
-      <c r="I24" s="56"/>
-      <c r="J24" s="56"/>
-      <c r="K24" s="57"/>
+      <c r="H24" s="110"/>
+      <c r="I24" s="111"/>
+      <c r="J24" s="111"/>
+      <c r="K24" s="112"/>
     </row>
     <row r="25" spans="2:11" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="65"/>
-      <c r="C25" s="66"/>
-      <c r="D25" s="67"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="38"/>
       <c r="E25" s="16"/>
       <c r="F25" s="15"/>
       <c r="G25" s="15"/>
-      <c r="H25" s="55"/>
-      <c r="I25" s="56"/>
-      <c r="J25" s="56"/>
-      <c r="K25" s="57"/>
+      <c r="H25" s="110"/>
+      <c r="I25" s="111"/>
+      <c r="J25" s="111"/>
+      <c r="K25" s="112"/>
     </row>
     <row r="26" spans="2:11" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="65"/>
-      <c r="C26" s="66"/>
-      <c r="D26" s="67"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="38"/>
       <c r="E26" s="16"/>
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
-      <c r="H26" s="55"/>
-      <c r="I26" s="56"/>
-      <c r="J26" s="56"/>
-      <c r="K26" s="57"/>
+      <c r="H26" s="110"/>
+      <c r="I26" s="111"/>
+      <c r="J26" s="111"/>
+      <c r="K26" s="112"/>
     </row>
     <row r="27" spans="2:11" s="4" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="119"/>
-      <c r="C27" s="120"/>
-      <c r="D27" s="121"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="41"/>
       <c r="E27" s="18"/>
       <c r="F27" s="19"/>
       <c r="G27" s="19"/>
-      <c r="H27" s="122"/>
-      <c r="I27" s="123"/>
-      <c r="J27" s="123"/>
-      <c r="K27" s="124"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="43"/>
+      <c r="J27" s="43"/>
+      <c r="K27" s="44"/>
     </row>
     <row r="28" spans="2:11" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B28" s="8"/>
@@ -2188,18 +2183,18 @@
       <c r="K28" s="8"/>
     </row>
     <row r="29" spans="2:11" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="43" t="s">
+      <c r="B29" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="44"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
-      <c r="K29" s="46"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="47"/>
+      <c r="H29" s="47"/>
+      <c r="I29" s="47"/>
+      <c r="J29" s="47"/>
+      <c r="K29" s="48"/>
     </row>
     <row r="30" spans="2:11" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="8"/>
@@ -2214,18 +2209,18 @@
       <c r="K30" s="8"/>
     </row>
     <row r="31" spans="2:11" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="43" t="s">
+      <c r="B31" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="44"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="45"/>
-      <c r="G31" s="45"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="45"/>
-      <c r="J31" s="45"/>
-      <c r="K31" s="46"/>
+      <c r="C31" s="46"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="47"/>
+      <c r="I31" s="47"/>
+      <c r="J31" s="47"/>
+      <c r="K31" s="48"/>
     </row>
     <row r="32" spans="2:11" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B32" s="9"/>
@@ -2240,27 +2235,27 @@
       <c r="K32" s="9"/>
     </row>
     <row r="33" spans="2:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="B33" s="125" t="s">
+      <c r="B33" s="49" t="s">
         <v>6</v>
       </c>
       <c r="C33" s="50"/>
-      <c r="D33" s="126"/>
+      <c r="D33" s="51"/>
       <c r="E33" s="9"/>
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
-      <c r="I33" s="127" t="s">
+      <c r="I33" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="J33" s="128"/>
-      <c r="K33" s="129"/>
+      <c r="J33" s="53"/>
+      <c r="K33" s="54"/>
     </row>
     <row r="34" spans="2:11" ht="15" x14ac:dyDescent="0.3">
       <c r="B34" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C34" s="34"/>
-      <c r="D34" s="35"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="33"/>
       <c r="E34" s="9"/>
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
@@ -2268,36 +2263,36 @@
       <c r="I34" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="J34" s="117"/>
-      <c r="K34" s="118"/>
+      <c r="J34" s="34"/>
+      <c r="K34" s="35"/>
     </row>
     <row r="35" spans="2:11" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B35" s="32" t="s">
+      <c r="B35" s="113" t="s">
         <v>4</v>
       </c>
-      <c r="C35" s="34"/>
-      <c r="D35" s="35"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="33"/>
       <c r="E35" s="9"/>
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
-      <c r="I35" s="32" t="s">
+      <c r="I35" s="113" t="s">
         <v>4</v>
       </c>
-      <c r="J35" s="34"/>
-      <c r="K35" s="35"/>
+      <c r="J35" s="32"/>
+      <c r="K35" s="33"/>
     </row>
     <row r="36" spans="2:11" ht="37.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="33"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="37"/>
+      <c r="B36" s="114"/>
+      <c r="C36" s="115"/>
+      <c r="D36" s="116"/>
       <c r="E36" s="10"/>
       <c r="F36" s="11"/>
       <c r="G36" s="11"/>
       <c r="H36" s="10"/>
-      <c r="I36" s="33"/>
-      <c r="J36" s="36"/>
-      <c r="K36" s="37"/>
+      <c r="I36" s="114"/>
+      <c r="J36" s="115"/>
+      <c r="K36" s="116"/>
     </row>
     <row r="37" spans="2:11" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="B37" s="3"/>
@@ -2338,48 +2333,6 @@
     <row r="40" spans="2:11" ht="13.8" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="H27:K27"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:K29"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="I33:K33"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B11:D12"/>
-    <mergeCell ref="B14:K14"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="D10:I10"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="D2:J4"/>
-    <mergeCell ref="B6:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D7:K7"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B2:C4"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="H23:K23"/>
-    <mergeCell ref="H24:K24"/>
-    <mergeCell ref="H25:K25"/>
-    <mergeCell ref="H26:K26"/>
-    <mergeCell ref="H18:K18"/>
-    <mergeCell ref="H19:K19"/>
-    <mergeCell ref="H20:K20"/>
-    <mergeCell ref="H21:K21"/>
-    <mergeCell ref="H22:K22"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
     <mergeCell ref="B35:B36"/>
     <mergeCell ref="C35:D36"/>
     <mergeCell ref="I35:I36"/>
@@ -2396,6 +2349,48 @@
     <mergeCell ref="H15:K15"/>
     <mergeCell ref="H17:K17"/>
     <mergeCell ref="D9:K9"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="H23:K23"/>
+    <mergeCell ref="H24:K24"/>
+    <mergeCell ref="H25:K25"/>
+    <mergeCell ref="H26:K26"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="H19:K19"/>
+    <mergeCell ref="H20:K20"/>
+    <mergeCell ref="H21:K21"/>
+    <mergeCell ref="H22:K22"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="D2:J4"/>
+    <mergeCell ref="B6:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D7:K7"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B2:C4"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B11:D12"/>
+    <mergeCell ref="B14:K14"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="D10:I10"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="H27:K27"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:K29"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="I33:K33"/>
   </mergeCells>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="94" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Se actualiza el servicio del excel de los mantenimientos
</commit_message>
<xml_diff>
--- a/src/main/resources/static/FO-GTI-01.xlsx
+++ b/src/main/resources/static/FO-GTI-01.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Inventario TI\inventory_system\src\main\resources\static\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cristian\IdeaProjects\inventory-system\src\main\resources\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7EA946-DB83-47EF-9FCD-2F4772B7DAD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0711BF1-F974-4286-970B-1A167BA52EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="267" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" tabRatio="267" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="2" r:id="rId1"/>
@@ -997,7 +997,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1197,12 +1197,6 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1347,13 +1341,13 @@
     <xf numFmtId="0" fontId="17" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1374,21 +1368,18 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1775,11 +1766,11 @@
   </sheetPr>
   <dimension ref="B1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:K8"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6:K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.6640625" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="21.6640625" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="0.5546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.33203125" style="1" customWidth="1"/>
@@ -1809,45 +1800,45 @@
       <c r="K1" s="2"/>
     </row>
     <row r="2" spans="2:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="99"/>
-      <c r="C2" s="100"/>
-      <c r="D2" s="79" t="s">
+      <c r="B2" s="97"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="81"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="79"/>
       <c r="K2" s="29" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="2:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="101"/>
-      <c r="C3" s="102"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="83"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
-      <c r="I3" s="83"/>
-      <c r="J3" s="84"/>
+      <c r="B3" s="99"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="82"/>
       <c r="K3" s="30" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="103"/>
-      <c r="C4" s="104"/>
-      <c r="D4" s="85"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
-      <c r="G4" s="86"/>
-      <c r="H4" s="86"/>
-      <c r="I4" s="86"/>
-      <c r="J4" s="87"/>
+      <c r="B4" s="101"/>
+      <c r="C4" s="102"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="84"/>
+      <c r="F4" s="84"/>
+      <c r="G4" s="84"/>
+      <c r="H4" s="84"/>
+      <c r="I4" s="84"/>
+      <c r="J4" s="85"/>
       <c r="K4" s="31" t="s">
         <v>28</v>
       </c>
@@ -1865,83 +1856,83 @@
       <c r="K5" s="10"/>
     </row>
     <row r="6" spans="2:12" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="88" t="s">
+      <c r="B6" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="89"/>
-      <c r="D6" s="76" t="s">
+      <c r="C6" s="87"/>
+      <c r="D6" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="77"/>
-      <c r="F6" s="69" t="s">
+      <c r="E6" s="75"/>
+      <c r="F6" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="69"/>
-      <c r="H6" s="70"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="68"/>
       <c r="I6" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="67"/>
-      <c r="K6" s="68"/>
+      <c r="J6" s="125"/>
+      <c r="K6" s="126"/>
     </row>
     <row r="7" spans="2:12" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="90"/>
-      <c r="C7" s="91"/>
-      <c r="D7" s="94" t="s">
+      <c r="B7" s="88"/>
+      <c r="C7" s="89"/>
+      <c r="D7" s="92" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="95"/>
-      <c r="F7" s="95"/>
-      <c r="G7" s="95"/>
-      <c r="H7" s="95"/>
-      <c r="I7" s="95"/>
-      <c r="J7" s="95"/>
-      <c r="K7" s="96"/>
+      <c r="E7" s="93"/>
+      <c r="F7" s="93"/>
+      <c r="G7" s="93"/>
+      <c r="H7" s="93"/>
+      <c r="I7" s="93"/>
+      <c r="J7" s="93"/>
+      <c r="K7" s="94"/>
     </row>
     <row r="8" spans="2:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="92" t="s">
+      <c r="B8" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="93"/>
-      <c r="D8" s="117"/>
-      <c r="E8" s="118"/>
-      <c r="F8" s="118"/>
-      <c r="G8" s="118"/>
-      <c r="H8" s="118"/>
-      <c r="I8" s="118"/>
-      <c r="J8" s="118"/>
-      <c r="K8" s="119"/>
+      <c r="C8" s="91"/>
+      <c r="D8" s="124"/>
+      <c r="E8" s="115"/>
+      <c r="F8" s="115"/>
+      <c r="G8" s="115"/>
+      <c r="H8" s="115"/>
+      <c r="I8" s="115"/>
+      <c r="J8" s="116"/>
+      <c r="K8" s="117"/>
       <c r="L8" s="4"/>
     </row>
     <row r="9" spans="2:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="105" t="s">
+      <c r="B9" s="103" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="106"/>
-      <c r="D9" s="126"/>
-      <c r="E9" s="127"/>
-      <c r="F9" s="127"/>
-      <c r="G9" s="127"/>
-      <c r="H9" s="127"/>
-      <c r="I9" s="127"/>
-      <c r="J9" s="128"/>
-      <c r="K9" s="129"/>
+      <c r="C9" s="104"/>
+      <c r="D9" s="124"/>
+      <c r="E9" s="115"/>
+      <c r="F9" s="115"/>
+      <c r="G9" s="115"/>
+      <c r="H9" s="115"/>
+      <c r="I9" s="115"/>
+      <c r="J9" s="116"/>
+      <c r="K9" s="117"/>
     </row>
     <row r="10" spans="2:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="97" t="s">
+      <c r="B10" s="95" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="98"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="74"/>
-      <c r="F10" s="74"/>
-      <c r="G10" s="74"/>
-      <c r="H10" s="74"/>
-      <c r="I10" s="75"/>
-      <c r="J10" s="71" t="s">
+      <c r="C10" s="96"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="72"/>
+      <c r="F10" s="72"/>
+      <c r="G10" s="72"/>
+      <c r="H10" s="72"/>
+      <c r="I10" s="73"/>
+      <c r="J10" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="K10" s="72"/>
+      <c r="K10" s="70"/>
     </row>
     <row r="11" spans="2:12" ht="15" x14ac:dyDescent="0.3">
       <c r="B11" s="58" t="s">
@@ -1949,7 +1940,7 @@
       </c>
       <c r="C11" s="59"/>
       <c r="D11" s="60"/>
-      <c r="E11" s="122" t="s">
+      <c r="E11" s="120" t="s">
         <v>7</v>
       </c>
       <c r="F11" s="50"/>
@@ -1969,10 +1960,10 @@
       <c r="B12" s="61"/>
       <c r="C12" s="62"/>
       <c r="D12" s="63"/>
-      <c r="E12" s="120"/>
-      <c r="F12" s="121"/>
-      <c r="G12" s="121"/>
-      <c r="H12" s="121"/>
+      <c r="E12" s="118"/>
+      <c r="F12" s="119"/>
+      <c r="G12" s="119"/>
+      <c r="H12" s="119"/>
       <c r="I12" s="25"/>
       <c r="J12" s="27" t="s">
         <v>30</v>
@@ -2005,11 +1996,11 @@
       <c r="K14" s="66"/>
     </row>
     <row r="15" spans="2:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="76" t="s">
+      <c r="B15" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="77"/>
-      <c r="D15" s="78"/>
+      <c r="C15" s="75"/>
+      <c r="D15" s="76"/>
       <c r="E15" s="22" t="s">
         <v>18</v>
       </c>
@@ -2019,12 +2010,12 @@
       <c r="G15" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="77" t="s">
+      <c r="H15" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="I15" s="77"/>
-      <c r="J15" s="77"/>
-      <c r="K15" s="78"/>
+      <c r="I15" s="75"/>
+      <c r="J15" s="75"/>
+      <c r="K15" s="76"/>
     </row>
     <row r="16" spans="2:12" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="55"/>
@@ -2033,22 +2024,22 @@
       <c r="E16" s="17"/>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
-      <c r="H16" s="123"/>
-      <c r="I16" s="124"/>
-      <c r="J16" s="124"/>
-      <c r="K16" s="125"/>
+      <c r="H16" s="121"/>
+      <c r="I16" s="122"/>
+      <c r="J16" s="122"/>
+      <c r="K16" s="123"/>
     </row>
     <row r="17" spans="2:11" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="107"/>
-      <c r="C17" s="108"/>
-      <c r="D17" s="109"/>
+      <c r="B17" s="105"/>
+      <c r="C17" s="106"/>
+      <c r="D17" s="107"/>
       <c r="E17" s="16"/>
       <c r="F17" s="15"/>
       <c r="G17" s="15"/>
-      <c r="H17" s="110"/>
-      <c r="I17" s="111"/>
-      <c r="J17" s="111"/>
-      <c r="K17" s="112"/>
+      <c r="H17" s="108"/>
+      <c r="I17" s="109"/>
+      <c r="J17" s="109"/>
+      <c r="K17" s="110"/>
     </row>
     <row r="18" spans="2:11" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="36"/>
@@ -2057,10 +2048,10 @@
       <c r="E18" s="16"/>
       <c r="F18" s="15"/>
       <c r="G18" s="15"/>
-      <c r="H18" s="110"/>
-      <c r="I18" s="111"/>
-      <c r="J18" s="111"/>
-      <c r="K18" s="112"/>
+      <c r="H18" s="108"/>
+      <c r="I18" s="109"/>
+      <c r="J18" s="109"/>
+      <c r="K18" s="110"/>
     </row>
     <row r="19" spans="2:11" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="36"/>
@@ -2069,10 +2060,10 @@
       <c r="E19" s="16"/>
       <c r="F19" s="15"/>
       <c r="G19" s="15"/>
-      <c r="H19" s="110"/>
-      <c r="I19" s="111"/>
-      <c r="J19" s="111"/>
-      <c r="K19" s="112"/>
+      <c r="H19" s="108"/>
+      <c r="I19" s="109"/>
+      <c r="J19" s="109"/>
+      <c r="K19" s="110"/>
     </row>
     <row r="20" spans="2:11" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="36"/>
@@ -2081,10 +2072,10 @@
       <c r="E20" s="16"/>
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>
-      <c r="H20" s="110"/>
-      <c r="I20" s="111"/>
-      <c r="J20" s="111"/>
-      <c r="K20" s="112"/>
+      <c r="H20" s="108"/>
+      <c r="I20" s="109"/>
+      <c r="J20" s="109"/>
+      <c r="K20" s="110"/>
     </row>
     <row r="21" spans="2:11" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="36"/>
@@ -2093,10 +2084,10 @@
       <c r="E21" s="16"/>
       <c r="F21" s="15"/>
       <c r="G21" s="15"/>
-      <c r="H21" s="110"/>
-      <c r="I21" s="111"/>
-      <c r="J21" s="111"/>
-      <c r="K21" s="112"/>
+      <c r="H21" s="108"/>
+      <c r="I21" s="109"/>
+      <c r="J21" s="109"/>
+      <c r="K21" s="110"/>
     </row>
     <row r="22" spans="2:11" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="36"/>
@@ -2105,10 +2096,10 @@
       <c r="E22" s="16"/>
       <c r="F22" s="15"/>
       <c r="G22" s="15"/>
-      <c r="H22" s="110"/>
-      <c r="I22" s="111"/>
-      <c r="J22" s="111"/>
-      <c r="K22" s="112"/>
+      <c r="H22" s="108"/>
+      <c r="I22" s="109"/>
+      <c r="J22" s="109"/>
+      <c r="K22" s="110"/>
     </row>
     <row r="23" spans="2:11" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="36"/>
@@ -2117,10 +2108,10 @@
       <c r="E23" s="16"/>
       <c r="F23" s="15"/>
       <c r="G23" s="15"/>
-      <c r="H23" s="110"/>
-      <c r="I23" s="111"/>
-      <c r="J23" s="111"/>
-      <c r="K23" s="112"/>
+      <c r="H23" s="108"/>
+      <c r="I23" s="109"/>
+      <c r="J23" s="109"/>
+      <c r="K23" s="110"/>
     </row>
     <row r="24" spans="2:11" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="36"/>
@@ -2129,10 +2120,10 @@
       <c r="E24" s="16"/>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
-      <c r="H24" s="110"/>
-      <c r="I24" s="111"/>
-      <c r="J24" s="111"/>
-      <c r="K24" s="112"/>
+      <c r="H24" s="108"/>
+      <c r="I24" s="109"/>
+      <c r="J24" s="109"/>
+      <c r="K24" s="110"/>
     </row>
     <row r="25" spans="2:11" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="36"/>
@@ -2141,10 +2132,10 @@
       <c r="E25" s="16"/>
       <c r="F25" s="15"/>
       <c r="G25" s="15"/>
-      <c r="H25" s="110"/>
-      <c r="I25" s="111"/>
-      <c r="J25" s="111"/>
-      <c r="K25" s="112"/>
+      <c r="H25" s="108"/>
+      <c r="I25" s="109"/>
+      <c r="J25" s="109"/>
+      <c r="K25" s="110"/>
     </row>
     <row r="26" spans="2:11" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="36"/>
@@ -2153,10 +2144,10 @@
       <c r="E26" s="16"/>
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
-      <c r="H26" s="110"/>
-      <c r="I26" s="111"/>
-      <c r="J26" s="111"/>
-      <c r="K26" s="112"/>
+      <c r="H26" s="108"/>
+      <c r="I26" s="109"/>
+      <c r="J26" s="109"/>
+      <c r="K26" s="110"/>
     </row>
     <row r="27" spans="2:11" s="4" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="39"/>
@@ -2267,7 +2258,7 @@
       <c r="K34" s="35"/>
     </row>
     <row r="35" spans="2:11" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B35" s="113" t="s">
+      <c r="B35" s="111" t="s">
         <v>4</v>
       </c>
       <c r="C35" s="32"/>
@@ -2276,23 +2267,23 @@
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
-      <c r="I35" s="113" t="s">
+      <c r="I35" s="111" t="s">
         <v>4</v>
       </c>
       <c r="J35" s="32"/>
       <c r="K35" s="33"/>
     </row>
     <row r="36" spans="2:11" ht="37.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="114"/>
-      <c r="C36" s="115"/>
-      <c r="D36" s="116"/>
+      <c r="B36" s="112"/>
+      <c r="C36" s="113"/>
+      <c r="D36" s="114"/>
       <c r="E36" s="10"/>
       <c r="F36" s="11"/>
       <c r="G36" s="11"/>
       <c r="H36" s="10"/>
-      <c r="I36" s="114"/>
-      <c r="J36" s="115"/>
-      <c r="K36" s="116"/>
+      <c r="I36" s="112"/>
+      <c r="J36" s="113"/>
+      <c r="K36" s="114"/>
     </row>
     <row r="37" spans="2:11" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="B37" s="3"/>

</xml_diff>